<commit_message>
resolved few warnings which actually can be ignored.
</commit_message>
<xml_diff>
--- a/config/Master_Test_Template.xlsx
+++ b/config/Master_Test_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A4952\PycharmProjects\april_automation_framework\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ETL Automation\ETL_Framework\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E204E9-4F7B-4684-9FC6-1C7F7700B91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE697FC7-3968-4039-B33D-BF86EBD0CE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_validation" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>name_check</t>
   </si>
   <si>
-    <t>contact_info_schema.json</t>
-  </si>
-  <si>
     <t>snowflake_db</t>
   </si>
   <si>
@@ -275,22 +272,32 @@
     <t>ETL_AUTO.CONTACT_INFO.CONTACT_INFO_BRONZE</t>
   </si>
   <si>
-    <t>contact_info_20240709.csv</t>
-  </si>
-  <si>
     <t>contact_info, transaction</t>
+  </si>
+  <si>
+    <t>E:\ETL Automation\ETL_Framework\files\Contact_info.csv</t>
+  </si>
+  <si>
+    <t>E:\ETL Automation\ETL_Framework\files\Contact_info_t.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -465,68 +472,71 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,6 +549,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -547,9 +566,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -829,10 +845,10 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -940,22 +956,22 @@
       <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>44</v>
+      <c r="F2" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>20</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="29" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -964,11 +980,11 @@
       <c r="M2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>22</v>
+      <c r="N2" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="P2" s="23" t="s">
         <v>21</v>
@@ -1008,17 +1024,17 @@
       <c r="F3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>44</v>
+      <c r="G3" s="29" t="s">
+        <v>20</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="K3" s="18" t="s">
         <v>20</v>
@@ -1029,11 +1045,11 @@
       <c r="M3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>22</v>
+      <c r="N3" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="P3" s="14" t="s">
         <v>21</v>
@@ -1073,17 +1089,17 @@
       <c r="F4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="21" t="s">
-        <v>44</v>
+      <c r="G4" s="29" t="s">
+        <v>20</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="K4" s="18" t="s">
         <v>20</v>
@@ -1094,11 +1110,11 @@
       <c r="M4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>22</v>
+      <c r="N4" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>21</v>
@@ -1138,17 +1154,17 @@
       <c r="F5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>44</v>
+      <c r="G5" s="29" t="s">
+        <v>20</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="K5" s="18" t="s">
         <v>20</v>
@@ -1159,11 +1175,11 @@
       <c r="M5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>22</v>
+      <c r="N5" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="P5" s="14" t="s">
         <v>21</v>
@@ -1203,17 +1219,17 @@
       <c r="F6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>44</v>
+      <c r="G6" s="29" t="s">
+        <v>20</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="K6" s="18" t="s">
         <v>20</v>
@@ -1224,11 +1240,11 @@
       <c r="M6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="13" t="s">
-        <v>22</v>
+      <c r="N6" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="P6" s="14" t="s">
         <v>21</v>
@@ -1268,17 +1284,17 @@
       <c r="F7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="21" t="s">
-        <v>44</v>
+      <c r="G7" s="29" t="s">
+        <v>20</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>20</v>
@@ -1289,11 +1305,11 @@
       <c r="M7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>22</v>
+      <c r="N7" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="O7" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="P7" s="14" t="s">
         <v>21</v>
@@ -1333,17 +1349,17 @@
       <c r="F8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="21" t="s">
-        <v>44</v>
+      <c r="G8" s="29" t="s">
+        <v>20</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="K8" s="18" t="s">
         <v>20</v>
@@ -1354,11 +1370,11 @@
       <c r="M8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>22</v>
+      <c r="N8" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="P8" s="14" t="s">
         <v>21</v>
@@ -1381,34 +1397,34 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K9" s="24" t="s">
         <v>20</v>
@@ -1429,7 +1445,7 @@
         <v>21</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>27</v>
@@ -1446,34 +1462,34 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="I10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K10" s="24" t="s">
         <v>20</v>
@@ -1494,7 +1510,7 @@
         <v>21</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>27</v>
@@ -1511,34 +1527,34 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="I11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K11" s="24" t="s">
         <v>20</v>
@@ -1559,7 +1575,7 @@
         <v>21</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>27</v>
@@ -1576,34 +1592,34 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="I12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K12" s="24" t="s">
         <v>20</v>
@@ -1624,7 +1640,7 @@
         <v>21</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>27</v>
@@ -1641,34 +1657,34 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="I13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" s="24" t="s">
         <v>20</v>
@@ -1689,7 +1705,7 @@
         <v>21</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>27</v>
@@ -1706,34 +1722,34 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="I14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K14" s="24" t="s">
         <v>20</v>
@@ -1754,7 +1770,7 @@
         <v>21</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="R14" s="2" t="s">
         <v>27</v>
@@ -1771,34 +1787,34 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="I15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K15" s="24" t="s">
         <v>20</v>
@@ -1819,7 +1835,7 @@
         <v>21</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="R15" s="2" t="s">
         <v>27</v>
@@ -1836,34 +1852,34 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="I16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K16" s="24" t="s">
         <v>20</v>
@@ -1884,7 +1900,7 @@
         <v>21</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>27</v>
@@ -1901,43 +1917,43 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="19" t="s">
+      <c r="I17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M17" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N17" s="26" t="s">
         <v>17</v>
@@ -1949,7 +1965,7 @@
         <v>21</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R17" s="2" t="s">
         <v>27</v>
@@ -1966,43 +1982,43 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="19" t="s">
+      <c r="I18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J18" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K18" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N18" s="26" t="s">
         <v>17</v>
@@ -2014,7 +2030,7 @@
         <v>21</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R18" s="2" t="s">
         <v>27</v>
@@ -2031,43 +2047,43 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="19" t="s">
+      <c r="I19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N19" s="26" t="s">
         <v>17</v>
@@ -2079,7 +2095,7 @@
         <v>21</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>27</v>
@@ -2096,43 +2112,43 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F20" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="19" t="s">
+      <c r="I20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J20" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M20" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N20" s="26" t="s">
         <v>17</v>
@@ -2144,7 +2160,7 @@
         <v>21</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>27</v>
@@ -2161,43 +2177,43 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="19" t="s">
+      <c r="I21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N21" s="26" t="s">
         <v>17</v>
@@ -2209,7 +2225,7 @@
         <v>21</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R21" s="2" t="s">
         <v>27</v>
@@ -2226,43 +2242,43 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F22" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="19" t="s">
+      <c r="I22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K22" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M22" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N22" s="26" t="s">
         <v>17</v>
@@ -2274,7 +2290,7 @@
         <v>21</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>27</v>
@@ -2291,43 +2307,43 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G23" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="19" t="s">
+      <c r="I23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K23" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K23" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M23" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N23" s="26" t="s">
         <v>17</v>
@@ -2339,7 +2355,7 @@
         <v>21</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R23" s="2" t="s">
         <v>27</v>
@@ -2356,43 +2372,43 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="19" t="s">
+      <c r="I24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K24" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M24" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N24" s="26" t="s">
         <v>17</v>
@@ -2404,7 +2420,7 @@
         <v>21</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R24" s="2" t="s">
         <v>27</v>
@@ -2421,43 +2437,43 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F25" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G25" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="19" t="s">
+      <c r="I25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K25" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M25" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N25" s="26" t="s">
         <v>17</v>
@@ -2469,10 +2485,10 @@
         <v>21</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S25" s="2" t="s">
         <v>27</v>
@@ -2486,43 +2502,43 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F26" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="19" t="s">
+      <c r="I26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J26" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K26" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M26" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N26" s="26" t="s">
         <v>17</v>
@@ -2534,10 +2550,10 @@
         <v>21</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S26" s="2" t="s">
         <v>27</v>
@@ -2551,43 +2567,43 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F27" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="19" t="s">
+      <c r="I27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K27" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M27" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N27" s="26" t="s">
         <v>17</v>
@@ -2599,10 +2615,10 @@
         <v>21</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R27" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S27" s="2" t="s">
         <v>27</v>
@@ -2616,43 +2632,43 @@
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F28" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="19" t="s">
+      <c r="I28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K28" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M28" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="N28" s="26" t="s">
         <v>17</v>
@@ -2664,13 +2680,13 @@
         <v>21</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="S28" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="T28" s="2">
         <v>0</v>
@@ -2683,7 +2699,7 @@
       <c r="A29" s="22"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -2798,7 +2814,7 @@
       <c r="Q34" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="20" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q34" xr:uid="{53648117-6315-BD4B-95C3-AF9A5887C458}">
       <formula1>"Y,N"</formula1>

</xml_diff>

<commit_message>
incorporated test.py for testing and improvised read_lib.py file by redefining read_csv and added a new function read_json to read json files
</commit_message>
<xml_diff>
--- a/config/Master_Test_Template.xlsx
+++ b/config/Master_Test_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ETL Automation\ETL_Framework\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE697FC7-3968-4039-B33D-BF86EBD0CE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BC6A2F-CD57-43A3-9F45-E09B57725793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="88">
   <si>
     <t>csv</t>
   </si>
@@ -279,18 +279,41 @@
   </si>
   <si>
     <t>E:\ETL Automation\ETL_Framework\files\Contact_info_t.csv</t>
+  </si>
+  <si>
+    <t>E:\ETL Automation\ETL_Framework\schema_files\Contact_info_schema.json</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>E:\ETL Automation\ETL_Framework\files\singleline.json</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -472,48 +495,67 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -521,19 +563,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -543,28 +572,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -845,10 +874,10 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -959,8 +988,8 @@
       <c r="F2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>20</v>
+      <c r="G2" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>84</v>
@@ -1024,8 +1053,8 @@
       <c r="F3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="29" t="s">
-        <v>20</v>
+      <c r="G3" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="H3" s="28" t="s">
         <v>84</v>
@@ -1089,8 +1118,8 @@
       <c r="F4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="29" t="s">
-        <v>20</v>
+      <c r="G4" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="H4" s="28" t="s">
         <v>84</v>
@@ -1154,8 +1183,8 @@
       <c r="F5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="29" t="s">
-        <v>20</v>
+      <c r="G5" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="H5" s="28" t="s">
         <v>84</v>
@@ -1219,8 +1248,8 @@
       <c r="F6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="29" t="s">
-        <v>20</v>
+      <c r="G6" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>84</v>
@@ -1284,8 +1313,8 @@
       <c r="F7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="29" t="s">
-        <v>20</v>
+      <c r="G7" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="H7" s="28" t="s">
         <v>84</v>
@@ -1338,25 +1367,25 @@
         <v>42</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="29" t="s">
+      <c r="F8" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="33" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="J8" s="20" t="s">
         <v>20</v>
@@ -2814,7 +2843,7 @@
       <c r="Q34" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="20" type="noConversion"/>
+  <phoneticPr fontId="22" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q34" xr:uid="{53648117-6315-BD4B-95C3-AF9A5887C458}">
       <formula1>"Y,N"</formula1>

</xml_diff>